<commit_message>
output de excel y pdf reporte ComposicionGnaLIV primera Quincena
</commit_message>
<xml_diff>
--- a/Unna.OperationalReport.WebSite/wwwroot/plantillas/reporte/quincenal/ComposicionQuincenalGNALoteIV.xlsx
+++ b/Unna.OperationalReport.WebSite/wwwroot/plantillas/reporte/quincenal/ComposicionQuincenalGNALoteIV.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27630"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\SP\UNNA-App\AppOperacionalReporte\UnnaReportesOperativos\Unna.OperationalReport.WebSite\wwwroot\plantillas\reporte\quincenal\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Desarrollos\SP\APSS SP\ProyectoPrincipalAenza5\UnnaReportesOperativos\Unna.OperationalReport.WebSite\wwwroot\plantillas\reporte\quincenal\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14ED8814-3CD9-4C0B-97A1-6AF649D01A3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{513E6233-9AE4-4065-8ED0-FD6C192EC964}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -24,21 +24,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
   <si>
     <t>COMPOSICION DE UNNA ENERGIA PROMEDIO MENSUAL (LOTE IV)</t>
   </si>
@@ -85,52 +76,85 @@
     <t>mol %</t>
   </si>
   <si>
-    <t>{{item.Fecha}}</t>
-  </si>
-  <si>
-    <t>{{item.C6}}</t>
-  </si>
-  <si>
-    <t>{{item.C3}}</t>
-  </si>
-  <si>
-    <t>{{item.Ic4}}</t>
-  </si>
-  <si>
-    <t>{{item.Nc4}}</t>
-  </si>
-  <si>
-    <t>{{item.NeoC5}}</t>
-  </si>
-  <si>
-    <t>{{item.Ic5}}</t>
-  </si>
-  <si>
-    <t>{{item.Observacion}}</t>
-  </si>
-  <si>
-    <t>{{item.C2}}</t>
-  </si>
-  <si>
-    <t>{{item.Co2}}</t>
-  </si>
-  <si>
-    <t>{{item.C1}}</t>
-  </si>
-  <si>
-    <t>{{item.Nitrog}}</t>
-  </si>
-  <si>
-    <t>{{item.Nc5}}</t>
-  </si>
-  <si>
-    <t>{{item.Simbolo}}</t>
-  </si>
-  <si>
-    <t>{{item.Componente}}</t>
-  </si>
-  <si>
-    <t>{{item.Molecula}}</t>
+    <t>{{item.CompGnaC6}}</t>
+  </si>
+  <si>
+    <t>{{item.CompGnaC3}}</t>
+  </si>
+  <si>
+    <t>{{item.CompGnaIc4}}</t>
+  </si>
+  <si>
+    <t>{{item.CompGnaNc4}}</t>
+  </si>
+  <si>
+    <t>{{item.CompGnaNeoC5}}</t>
+  </si>
+  <si>
+    <t>{{item.CompGnaIc5}}</t>
+  </si>
+  <si>
+    <t>{{item.CompGnaNc5}}</t>
+  </si>
+  <si>
+    <t>{{item.CompGnaNitrog}}</t>
+  </si>
+  <si>
+    <t>{{item.CompGnaC1}}</t>
+  </si>
+  <si>
+    <t>{{item.CompGnaCo2}}</t>
+  </si>
+  <si>
+    <t>{{item.CompGnaC2}}</t>
+  </si>
+  <si>
+    <t>{{item.CompGnaObservacion}}</t>
+  </si>
+  <si>
+    <t>{{item.CompGnaDia}}</t>
+  </si>
+  <si>
+    <t>{{item.CompSimbolo}}</t>
+  </si>
+  <si>
+    <t>{{item.CompDescripcion}}</t>
+  </si>
+  <si>
+    <t>{{item.CompMolPorc}}</t>
+  </si>
+  <si>
+    <t>{{TotalPromedioPeruPetroC6}}</t>
+  </si>
+  <si>
+    <t>{{TotalPromedioPeruPetroC3}}</t>
+  </si>
+  <si>
+    <t>{{TotalPromedioPeruPetroNeoC5}}</t>
+  </si>
+  <si>
+    <t>{{TotalPromedioPeruPetroIc5}}</t>
+  </si>
+  <si>
+    <t>{{TotalPromedioPeruPetroNc5}}</t>
+  </si>
+  <si>
+    <t>{{TotalPromedioPeruPetroNitrog}}</t>
+  </si>
+  <si>
+    <t>{{TotalPromedioPeruPetroC1}}</t>
+  </si>
+  <si>
+    <t>{{TotalPromedioPeruPetroCo2}}</t>
+  </si>
+  <si>
+    <t>{{TotalPromedioPeruPetroC2}}</t>
+  </si>
+  <si>
+    <t>{{TotalPromedioPeruPetroNc4}}</t>
+  </si>
+  <si>
+    <t>{{TotalPromedioPeruPetroIc4}}</t>
   </si>
 </sst>
 </file>
@@ -530,7 +554,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
     <xf numFmtId="170" fontId="9" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -540,9 +564,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="169" fontId="7" fillId="4" borderId="0" xfId="103" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -593,7 +614,7 @@
     <xf numFmtId="14" fontId="0" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="7" fillId="5" borderId="1" xfId="104" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1059,36 +1080,36 @@
   <dimension ref="A1:Q11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H38" sqref="H38"/>
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="1.42578125" customWidth="1"/>
-    <col min="2" max="2" width="12.7109375" customWidth="1"/>
-    <col min="3" max="13" width="9.85546875" customWidth="1"/>
-    <col min="14" max="14" width="19.7109375" customWidth="1"/>
+    <col min="1" max="1" width="1.44140625" customWidth="1"/>
+    <col min="2" max="2" width="12.6640625" customWidth="1"/>
+    <col min="3" max="13" width="9.88671875" customWidth="1"/>
+    <col min="14" max="14" width="19.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C1" s="26" t="s">
+    <row r="1" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C1" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
-      <c r="F1" s="27"/>
-      <c r="G1" s="27"/>
-      <c r="H1" s="27"/>
-      <c r="I1" s="27"/>
-      <c r="J1" s="27"/>
-      <c r="K1" s="27"/>
-      <c r="L1" s="27"/>
-      <c r="M1" s="27"/>
-      <c r="N1" s="28"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="26"/>
+      <c r="H1" s="26"/>
+      <c r="I1" s="26"/>
+      <c r="J1" s="26"/>
+      <c r="K1" s="26"/>
+      <c r="L1" s="26"/>
+      <c r="M1" s="26"/>
+      <c r="N1" s="27"/>
     </row>
-    <row r="2" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="10"/>
+    <row r="2" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B2" s="9"/>
       <c r="C2" s="1" t="s">
         <v>1</v>
       </c>
@@ -1126,173 +1147,196 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="10"/>
-      <c r="B3" s="22" t="s">
+    <row r="3" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="9"/>
+      <c r="B3" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="C3" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="19" t="s">
+      <c r="D3" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="D3" s="19" t="s">
+      <c r="E3" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="E3" s="19" t="s">
+      <c r="F3" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="F3" s="19" t="s">
+      <c r="G3" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="G3" s="19" t="s">
+      <c r="H3" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="H3" s="19" t="s">
+      <c r="I3" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="I3" s="19" t="s">
-        <v>27</v>
-      </c>
-      <c r="J3" s="19" t="s">
+      <c r="J3" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="K3" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="L3" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="M3" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="N3" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="K3" s="19" t="s">
-        <v>25</v>
-      </c>
-      <c r="L3" s="19" t="s">
-        <v>24</v>
-      </c>
-      <c r="M3" s="19" t="s">
-        <v>23</v>
-      </c>
-      <c r="N3" s="20" t="s">
-        <v>22</v>
-      </c>
-      <c r="O3" s="14"/>
+      <c r="O3" s="13"/>
     </row>
-    <row r="4" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="10"/>
-      <c r="B4" s="23"/>
-      <c r="C4" s="19"/>
-      <c r="D4" s="19"/>
-      <c r="E4" s="19"/>
-      <c r="F4" s="19"/>
-      <c r="G4" s="19"/>
-      <c r="H4" s="19"/>
-      <c r="I4" s="19"/>
-      <c r="J4" s="19"/>
-      <c r="K4" s="19"/>
-      <c r="L4" s="19"/>
-      <c r="M4" s="19"/>
-      <c r="N4" s="21"/>
-      <c r="O4" s="14"/>
+    <row r="4" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="9"/>
+      <c r="B4" s="22"/>
+      <c r="C4" s="18"/>
+      <c r="D4" s="18"/>
+      <c r="E4" s="18"/>
+      <c r="F4" s="18"/>
+      <c r="G4" s="18"/>
+      <c r="H4" s="18"/>
+      <c r="I4" s="18"/>
+      <c r="J4" s="18"/>
+      <c r="K4" s="18"/>
+      <c r="L4" s="18"/>
+      <c r="M4" s="18"/>
+      <c r="N4" s="20"/>
+      <c r="O4" s="13"/>
     </row>
-    <row r="5" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="10"/>
-      <c r="B5" s="9"/>
-      <c r="C5" s="11"/>
-      <c r="D5" s="12"/>
-      <c r="E5" s="12"/>
-      <c r="F5" s="12"/>
-      <c r="G5" s="13"/>
-      <c r="H5" s="13"/>
-      <c r="I5" s="13"/>
-      <c r="J5" s="13"/>
-      <c r="K5" s="13"/>
-      <c r="L5" s="13"/>
-      <c r="M5" s="15"/>
-      <c r="N5" s="16"/>
-      <c r="O5" s="14"/>
+    <row r="5" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="9"/>
+      <c r="B5" s="8"/>
+      <c r="C5" s="10"/>
+      <c r="D5" s="11"/>
+      <c r="E5" s="11"/>
+      <c r="F5" s="11"/>
+      <c r="G5" s="12"/>
+      <c r="H5" s="12"/>
+      <c r="I5" s="12"/>
+      <c r="J5" s="12"/>
+      <c r="K5" s="12"/>
+      <c r="L5" s="12"/>
+      <c r="M5" s="14"/>
+      <c r="N5" s="15"/>
+      <c r="O5" s="13"/>
     </row>
-    <row r="6" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="4"/>
-      <c r="H6" s="4"/>
-      <c r="I6" s="4"/>
-      <c r="J6" s="4"/>
-      <c r="K6" s="4"/>
-      <c r="L6" s="4"/>
-      <c r="M6" s="4"/>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="C6" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="D6" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="E6" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="F6" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="G6" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="H6" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="I6" s="18" t="s">
+        <v>35</v>
+      </c>
+      <c r="J6" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="K6" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="L6" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="M6" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="N6" s="19"/>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="C7" s="24"/>
-      <c r="D7" s="24"/>
-      <c r="E7" s="24"/>
-      <c r="F7" s="24"/>
-      <c r="G7" s="24"/>
-      <c r="H7" s="24"/>
-      <c r="I7" s="24"/>
-      <c r="J7" s="24"/>
-      <c r="K7" s="24"/>
-      <c r="L7" s="24"/>
-      <c r="M7" s="24"/>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="C7" s="23"/>
+      <c r="D7" s="23"/>
+      <c r="E7" s="23"/>
+      <c r="F7" s="23"/>
+      <c r="G7" s="23"/>
+      <c r="H7" s="23"/>
+      <c r="I7" s="23"/>
+      <c r="J7" s="23"/>
+      <c r="K7" s="23"/>
+      <c r="L7" s="23"/>
+      <c r="M7" s="23"/>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="C8" s="14"/>
-      <c r="D8" s="14"/>
-      <c r="E8" s="14"/>
-      <c r="F8" s="14"/>
-      <c r="G8" s="14"/>
-      <c r="H8" s="14"/>
-      <c r="I8" s="14"/>
-      <c r="J8" s="14"/>
-      <c r="K8" s="14"/>
-      <c r="L8" s="14"/>
-      <c r="M8" s="14"/>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="C8" s="13"/>
+      <c r="D8" s="13"/>
+      <c r="E8" s="13"/>
+      <c r="F8" s="13"/>
+      <c r="G8" s="13"/>
+      <c r="H8" s="13"/>
+      <c r="I8" s="13"/>
+      <c r="J8" s="13"/>
+      <c r="K8" s="13"/>
+      <c r="L8" s="13"/>
+      <c r="M8" s="13"/>
     </row>
-    <row r="9" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="5"/>
-      <c r="C9" s="31" t="s">
+    <row r="9" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B9" s="4"/>
+      <c r="C9" s="30" t="s">
         <v>13</v>
       </c>
-      <c r="D9" s="31"/>
-      <c r="E9" s="6" t="s">
+      <c r="D9" s="30"/>
+      <c r="E9" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F9" s="17"/>
-      <c r="G9" s="18"/>
-      <c r="H9" s="18"/>
-      <c r="I9" s="18"/>
-      <c r="J9" s="18"/>
-      <c r="K9" s="18"/>
-      <c r="L9" s="18"/>
-      <c r="M9" s="18"/>
-      <c r="N9" s="18"/>
-      <c r="O9" s="18"/>
-      <c r="P9" s="18"/>
-      <c r="Q9" s="18"/>
+      <c r="F9" s="16"/>
+      <c r="G9" s="17"/>
+      <c r="H9" s="17"/>
+      <c r="I9" s="17"/>
+      <c r="J9" s="17"/>
+      <c r="K9" s="17"/>
+      <c r="L9" s="17"/>
+      <c r="M9" s="17"/>
+      <c r="N9" s="17"/>
+      <c r="O9" s="17"/>
+      <c r="P9" s="17"/>
+      <c r="Q9" s="17"/>
     </row>
-    <row r="10" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="7" t="s">
+    <row r="10" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B10" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="C10" s="29" t="s">
+      <c r="C10" s="28" t="s">
         <v>29</v>
       </c>
-      <c r="D10" s="30"/>
-      <c r="E10" s="25" t="s">
+      <c r="D10" s="29"/>
+      <c r="E10" s="24" t="s">
         <v>30</v>
       </c>
-      <c r="F10" s="17"/>
-      <c r="G10" s="18"/>
-      <c r="H10" s="18"/>
-      <c r="I10" s="18"/>
-      <c r="J10" s="18"/>
-      <c r="K10" s="18"/>
-      <c r="L10" s="18"/>
-      <c r="M10" s="18"/>
-      <c r="N10" s="18"/>
-      <c r="O10" s="18"/>
-      <c r="P10" s="18"/>
-      <c r="Q10" s="18"/>
+      <c r="F10" s="16"/>
+      <c r="G10" s="17"/>
+      <c r="H10" s="17"/>
+      <c r="I10" s="17"/>
+      <c r="J10" s="17"/>
+      <c r="K10" s="17"/>
+      <c r="L10" s="17"/>
+      <c r="M10" s="17"/>
+      <c r="N10" s="17"/>
+      <c r="O10" s="17"/>
+      <c r="P10" s="17"/>
+      <c r="Q10" s="17"/>
     </row>
-    <row r="11" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="7"/>
-      <c r="C11" s="29"/>
-      <c r="D11" s="30"/>
-      <c r="E11" s="8"/>
+    <row r="11" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B11" s="6"/>
+      <c r="C11" s="28"/>
+      <c r="D11" s="29"/>
+      <c r="E11" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>

<commit_message>
exportar en pdf en una sola hoja. Tamaño  de Hoja
</commit_message>
<xml_diff>
--- a/Unna.OperationalReport.WebSite/wwwroot/plantillas/reporte/quincenal/ComposicionQuincenalGNALoteIV.xlsx
+++ b/Unna.OperationalReport.WebSite/wwwroot/plantillas/reporte/quincenal/ComposicionQuincenalGNALoteIV.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27630"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27715"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Desarrollos\SP\APSS SP\ProyectoPrincipalAenza5\UnnaReportesOperativos\Unna.OperationalReport.WebSite\wwwroot\plantillas\reporte\quincenal\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{513E6233-9AE4-4065-8ED0-FD6C192EC964}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8259A14D-8458-42E9-ACB5-3761C22EA517}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="Componente_Items">Hoja1!$B$10:$E$11</definedName>
+    <definedName name="Componente_Items">Hoja1!$B$8:$E$9</definedName>
     <definedName name="Composicion_Items">Hoja1!$B$3:$N$4</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
@@ -173,7 +173,7 @@
     <numFmt numFmtId="171" formatCode="0.0000_ ;[Red]\-0.0000\ "/>
     <numFmt numFmtId="172" formatCode="0.0000000000_ ;[Red]\-0.0000000000\ "/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -208,33 +208,54 @@
       <scheme val="major"/>
     </font>
     <font>
+      <sz val="10"/>
+      <name val="Helvetica"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="Helvetica"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="11"/>
+      <sz val="12"/>
       <color theme="0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Helvetica"/>
+      <sz val="12"/>
+      <name val="Calibri Light"/>
       <family val="2"/>
+      <scheme val="major"/>
     </font>
     <font>
-      <sz val="9"/>
-      <name val="Arial"/>
+      <sz val="12"/>
+      <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="9"/>
-      <name val="Arial"/>
+      <sz val="12"/>
+      <name val="Calibri"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <name val="Helvetica"/>
-      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="6">
@@ -269,7 +290,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="14">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -317,16 +338,55 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="medium">
         <color indexed="64"/>
       </left>
       <right style="medium">
         <color indexed="64"/>
       </right>
-      <top style="thin">
+      <top style="medium">
         <color indexed="64"/>
       </top>
       <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -336,64 +396,10 @@
       <right style="medium">
         <color indexed="64"/>
       </right>
-      <top style="thin">
+      <top style="medium">
         <color indexed="64"/>
       </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
       <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -403,10 +409,32 @@
       <right style="medium">
         <color indexed="64"/>
       </right>
-      <top style="medium">
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom style="medium">
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -415,34 +443,12 @@
       <left style="medium">
         <color indexed="64"/>
       </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
       <right style="medium">
         <color indexed="64"/>
       </right>
       <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
       <bottom/>
       <diagonal/>
     </border>
@@ -551,91 +557,96 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="168" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
-    <xf numFmtId="170" fontId="9" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
+    <xf numFmtId="170" fontId="6" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="169" fontId="7" fillId="4" borderId="0" xfId="103" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="7" fillId="4" borderId="0" xfId="103" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" xfId="103" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="7" fillId="5" borderId="8" xfId="104" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="171" fontId="4" fillId="2" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="171" fontId="4" fillId="2" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="171" fontId="4" fillId="2" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="171" fontId="4" fillId="2" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="171" fontId="4" fillId="2" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="171" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="171" fontId="4" fillId="2" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="172" fontId="4" fillId="2" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="172" fontId="4" fillId="2" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="7" fillId="5" borderId="1" xfId="104" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="169" fontId="7" fillId="0" borderId="0" xfId="103" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="13" xfId="103" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="169" fontId="8" fillId="4" borderId="0" xfId="103" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="7" fillId="5" borderId="7" xfId="104" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="8" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="171" fontId="10" fillId="2" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="172" fontId="10" fillId="2" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="8" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="11" fillId="0" borderId="0" xfId="103" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="11" fillId="5" borderId="1" xfId="104" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="11" fillId="4" borderId="0" xfId="103" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="11" fillId="4" borderId="0" xfId="103" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="11" fillId="0" borderId="0" xfId="103" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="11" fillId="0" borderId="9" xfId="103" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="12" fillId="4" borderId="0" xfId="103" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" xfId="103" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="9" xfId="103" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="171" fontId="10" fillId="2" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="172" fontId="10" fillId="2" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="172" fontId="10" fillId="2" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="171" fontId="10" fillId="2" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -765,13 +776,13 @@
     <xdr:from>
       <xdr:col>7</xdr:col>
       <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>30</xdr:row>
+      <xdr:row>28</xdr:row>
       <xdr:rowOff>38101</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>333375</xdr:colOff>
-      <xdr:row>35</xdr:row>
+      <xdr:row>33</xdr:row>
       <xdr:rowOff>59240</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1077,11 +1088,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q11"/>
+  <dimension ref="A1:Q9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I6" sqref="I6"/>
+      <selection pane="bottomLeft" activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1092,258 +1103,230 @@
     <col min="14" max="14" width="19.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C1" s="25" t="s">
+    <row r="1" spans="1:17" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B1" s="8"/>
+      <c r="C1" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
-      <c r="F1" s="26"/>
-      <c r="G1" s="26"/>
-      <c r="H1" s="26"/>
-      <c r="I1" s="26"/>
-      <c r="J1" s="26"/>
-      <c r="K1" s="26"/>
-      <c r="L1" s="26"/>
-      <c r="M1" s="26"/>
-      <c r="N1" s="27"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="22"/>
+      <c r="I1" s="22"/>
+      <c r="J1" s="22"/>
+      <c r="K1" s="22"/>
+      <c r="L1" s="22"/>
+      <c r="M1" s="22"/>
+      <c r="N1" s="23"/>
     </row>
-    <row r="2" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="9"/>
-      <c r="C2" s="1" t="s">
+    <row r="2" spans="1:17" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B2" s="11"/>
+      <c r="C2" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="G2" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="H2" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="I2" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="J2" s="3" t="s">
+      <c r="J2" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="K2" s="3" t="s">
+      <c r="K2" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="L2" s="3" t="s">
+      <c r="L2" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="M2" s="3" t="s">
+      <c r="M2" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="N2" s="3" t="s">
+      <c r="N2" s="12" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="9"/>
-      <c r="B3" s="21" t="s">
+    <row r="3" spans="1:17" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="1"/>
+      <c r="B3" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="C3" s="18" t="s">
+      <c r="C3" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="D3" s="18" t="s">
+      <c r="D3" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="E3" s="18" t="s">
+      <c r="E3" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="F3" s="18" t="s">
+      <c r="F3" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="G3" s="18" t="s">
+      <c r="G3" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="H3" s="18" t="s">
+      <c r="H3" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="I3" s="18" t="s">
+      <c r="I3" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="J3" s="18" t="s">
+      <c r="J3" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="K3" s="18" t="s">
+      <c r="K3" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="L3" s="18" t="s">
+      <c r="L3" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="M3" s="18" t="s">
+      <c r="M3" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="N3" s="19" t="s">
+      <c r="N3" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="O3" s="13"/>
+      <c r="O3" s="2"/>
     </row>
-    <row r="4" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="9"/>
-      <c r="B4" s="22"/>
-      <c r="C4" s="18"/>
-      <c r="D4" s="18"/>
-      <c r="E4" s="18"/>
-      <c r="F4" s="18"/>
-      <c r="G4" s="18"/>
-      <c r="H4" s="18"/>
-      <c r="I4" s="18"/>
-      <c r="J4" s="18"/>
-      <c r="K4" s="18"/>
-      <c r="L4" s="18"/>
-      <c r="M4" s="18"/>
-      <c r="N4" s="20"/>
-      <c r="O4" s="13"/>
+    <row r="4" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A4" s="1"/>
+      <c r="B4" s="16"/>
+      <c r="C4" s="14"/>
+      <c r="D4" s="14"/>
+      <c r="E4" s="14"/>
+      <c r="F4" s="14"/>
+      <c r="G4" s="14"/>
+      <c r="H4" s="14"/>
+      <c r="I4" s="14"/>
+      <c r="J4" s="14"/>
+      <c r="K4" s="14"/>
+      <c r="L4" s="14"/>
+      <c r="M4" s="14"/>
+      <c r="N4" s="30"/>
+      <c r="O4" s="2"/>
     </row>
-    <row r="5" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="9"/>
-      <c r="B5" s="8"/>
-      <c r="C5" s="10"/>
-      <c r="D5" s="11"/>
-      <c r="E5" s="11"/>
-      <c r="F5" s="11"/>
-      <c r="G5" s="12"/>
-      <c r="H5" s="12"/>
-      <c r="I5" s="12"/>
-      <c r="J5" s="12"/>
-      <c r="K5" s="12"/>
-      <c r="L5" s="12"/>
-      <c r="M5" s="14"/>
-      <c r="N5" s="15"/>
-      <c r="O5" s="13"/>
+    <row r="5" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B5" s="32"/>
+      <c r="C5" s="33" t="s">
+        <v>31</v>
+      </c>
+      <c r="D5" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="E5" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="F5" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="G5" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="H5" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="I5" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="J5" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="K5" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="L5" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="M5" s="29" t="s">
+        <v>39</v>
+      </c>
+      <c r="N5" s="31"/>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="C6" s="18" t="s">
-        <v>31</v>
-      </c>
-      <c r="D6" s="18" t="s">
-        <v>32</v>
-      </c>
-      <c r="E6" s="18" t="s">
-        <v>41</v>
-      </c>
-      <c r="F6" s="18" t="s">
-        <v>40</v>
-      </c>
-      <c r="G6" s="18" t="s">
-        <v>33</v>
-      </c>
-      <c r="H6" s="18" t="s">
-        <v>34</v>
-      </c>
-      <c r="I6" s="18" t="s">
-        <v>35</v>
-      </c>
-      <c r="J6" s="18" t="s">
-        <v>36</v>
-      </c>
-      <c r="K6" s="18" t="s">
-        <v>37</v>
-      </c>
-      <c r="L6" s="18" t="s">
-        <v>38</v>
-      </c>
-      <c r="M6" s="18" t="s">
-        <v>39</v>
-      </c>
-      <c r="N6" s="19"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="5"/>
+      <c r="H6" s="5"/>
+      <c r="I6" s="5"/>
+      <c r="J6" s="5"/>
+      <c r="K6" s="5"/>
+      <c r="L6" s="5"/>
+      <c r="M6" s="5"/>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="C7" s="23"/>
-      <c r="D7" s="23"/>
-      <c r="E7" s="23"/>
-      <c r="F7" s="23"/>
-      <c r="G7" s="23"/>
-      <c r="H7" s="23"/>
-      <c r="I7" s="23"/>
-      <c r="J7" s="23"/>
-      <c r="K7" s="23"/>
-      <c r="L7" s="23"/>
-      <c r="M7" s="23"/>
+    <row r="7" spans="1:17" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B7" s="19"/>
+      <c r="C7" s="26" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" s="26"/>
+      <c r="E7" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="F7" s="3"/>
+      <c r="G7" s="4"/>
+      <c r="H7" s="4"/>
+      <c r="I7" s="4"/>
+      <c r="J7" s="4"/>
+      <c r="K7" s="4"/>
+      <c r="L7" s="4"/>
+      <c r="M7" s="4"/>
+      <c r="N7" s="4"/>
+      <c r="O7" s="4"/>
+      <c r="P7" s="4"/>
+      <c r="Q7" s="4"/>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="C8" s="13"/>
-      <c r="D8" s="13"/>
-      <c r="E8" s="13"/>
-      <c r="F8" s="13"/>
-      <c r="G8" s="13"/>
-      <c r="H8" s="13"/>
-      <c r="I8" s="13"/>
-      <c r="J8" s="13"/>
-      <c r="K8" s="13"/>
-      <c r="L8" s="13"/>
-      <c r="M8" s="13"/>
+    <row r="8" spans="1:17" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B8" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="C8" s="24" t="s">
+        <v>29</v>
+      </c>
+      <c r="D8" s="25"/>
+      <c r="E8" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="F8" s="3"/>
+      <c r="G8" s="4"/>
+      <c r="H8" s="4"/>
+      <c r="I8" s="4"/>
+      <c r="J8" s="4"/>
+      <c r="K8" s="4"/>
+      <c r="L8" s="4"/>
+      <c r="M8" s="4"/>
+      <c r="N8" s="4"/>
+      <c r="O8" s="4"/>
+      <c r="P8" s="4"/>
+      <c r="Q8" s="4"/>
     </row>
     <row r="9" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B9" s="4"/>
-      <c r="C9" s="30" t="s">
-        <v>13</v>
-      </c>
-      <c r="D9" s="30"/>
-      <c r="E9" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="F9" s="16"/>
-      <c r="G9" s="17"/>
-      <c r="H9" s="17"/>
-      <c r="I9" s="17"/>
-      <c r="J9" s="17"/>
-      <c r="K9" s="17"/>
-      <c r="L9" s="17"/>
-      <c r="M9" s="17"/>
-      <c r="N9" s="17"/>
-      <c r="O9" s="17"/>
-      <c r="P9" s="17"/>
-      <c r="Q9" s="17"/>
-    </row>
-    <row r="10" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B10" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="C10" s="28" t="s">
-        <v>29</v>
-      </c>
-      <c r="D10" s="29"/>
-      <c r="E10" s="24" t="s">
-        <v>30</v>
-      </c>
-      <c r="F10" s="16"/>
-      <c r="G10" s="17"/>
-      <c r="H10" s="17"/>
-      <c r="I10" s="17"/>
-      <c r="J10" s="17"/>
-      <c r="K10" s="17"/>
-      <c r="L10" s="17"/>
-      <c r="M10" s="17"/>
-      <c r="N10" s="17"/>
-      <c r="O10" s="17"/>
-      <c r="P10" s="17"/>
-      <c r="Q10" s="17"/>
-    </row>
-    <row r="11" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B11" s="6"/>
-      <c r="C11" s="28"/>
-      <c r="D11" s="29"/>
-      <c r="E11" s="7"/>
+      <c r="B9" s="6"/>
+      <c r="C9" s="27"/>
+      <c r="D9" s="28"/>
+      <c r="E9" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="C1:N1"/>
-    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="C7:D7"/>
     <mergeCell ref="C9:D9"/>
-    <mergeCell ref="C11:D11"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" horizontalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
Reporte de Compensacion mensual, Sumistro GNS LIVa enel los botones de pdf excel y guardar sin que actualice aun , y avances del reporte anexo 7
</commit_message>
<xml_diff>
--- a/Unna.OperationalReport.WebSite/wwwroot/plantillas/reporte/quincenal/ComposicionQuincenalGNALoteIV.xlsx
+++ b/Unna.OperationalReport.WebSite/wwwroot/plantillas/reporte/quincenal/ComposicionQuincenalGNALoteIV.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Desarrollos\SP\APSS SP\ProyectoPrincipalAenza5\UnnaReportesOperativos\Unna.OperationalReport.WebSite\wwwroot\plantillas\reporte\quincenal\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8259A14D-8458-42E9-ACB5-3761C22EA517}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD7E54C4-FF07-4398-A34A-031763C701F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -173,7 +173,7 @@
     <numFmt numFmtId="171" formatCode="0.0000_ ;[Red]\-0.0000\ "/>
     <numFmt numFmtId="172" formatCode="0.0000000000_ ;[Red]\-0.0000000000\ "/>
   </numFmts>
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -253,6 +253,21 @@
     <font>
       <b/>
       <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <name val="Calibri Light"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -560,7 +575,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
     <xf numFmtId="170" fontId="6" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -588,9 +603,6 @@
     <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="8" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="171" fontId="10" fillId="2" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -603,15 +615,31 @@
     <xf numFmtId="169" fontId="11" fillId="0" borderId="0" xfId="103" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="11" fillId="5" borderId="1" xfId="104" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="169" fontId="11" fillId="4" borderId="0" xfId="103" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="11" fillId="4" borderId="0" xfId="103" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="172" fontId="10" fillId="2" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="172" fontId="10" fillId="2" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="171" fontId="13" fillId="2" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="171" fontId="13" fillId="2" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="171" fontId="13" fillId="2" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="14" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -636,17 +664,7 @@
     <xf numFmtId="169" fontId="7" fillId="0" borderId="9" xfId="103" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="171" fontId="10" fillId="2" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="172" fontId="10" fillId="2" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="172" fontId="10" fillId="2" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="171" fontId="10" fillId="2" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="12" fillId="5" borderId="1" xfId="104" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1092,7 +1110,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D5" sqref="D5"/>
+      <selection pane="bottomLeft" activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1105,20 +1123,20 @@
   <sheetData>
     <row r="1" spans="1:17" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B1" s="8"/>
-      <c r="C1" s="21" t="s">
+      <c r="C1" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
-      <c r="G1" s="22"/>
-      <c r="H1" s="22"/>
-      <c r="I1" s="22"/>
-      <c r="J1" s="22"/>
-      <c r="K1" s="22"/>
-      <c r="L1" s="22"/>
-      <c r="M1" s="22"/>
-      <c r="N1" s="23"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
+      <c r="F1" s="27"/>
+      <c r="G1" s="27"/>
+      <c r="H1" s="27"/>
+      <c r="I1" s="27"/>
+      <c r="J1" s="27"/>
+      <c r="K1" s="27"/>
+      <c r="L1" s="27"/>
+      <c r="M1" s="27"/>
+      <c r="N1" s="28"/>
     </row>
     <row r="2" spans="1:17" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B2" s="11"/>
@@ -1161,100 +1179,100 @@
     </row>
     <row r="3" spans="1:17" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="1"/>
-      <c r="B3" s="13" t="s">
+      <c r="B3" s="25" t="s">
         <v>27</v>
       </c>
-      <c r="C3" s="14" t="s">
+      <c r="C3" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="D3" s="14" t="s">
+      <c r="D3" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="E3" s="14" t="s">
+      <c r="E3" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="F3" s="14" t="s">
+      <c r="F3" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="G3" s="14" t="s">
+      <c r="G3" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="H3" s="14" t="s">
+      <c r="H3" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="I3" s="14" t="s">
+      <c r="I3" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="J3" s="14" t="s">
+      <c r="J3" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="K3" s="14" t="s">
+      <c r="K3" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="L3" s="14" t="s">
+      <c r="L3" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="M3" s="14" t="s">
+      <c r="M3" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="N3" s="15" t="s">
+      <c r="N3" s="14" t="s">
         <v>26</v>
       </c>
       <c r="O3" s="2"/>
     </row>
     <row r="4" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
-      <c r="B4" s="16"/>
-      <c r="C4" s="14"/>
-      <c r="D4" s="14"/>
-      <c r="E4" s="14"/>
-      <c r="F4" s="14"/>
-      <c r="G4" s="14"/>
-      <c r="H4" s="14"/>
-      <c r="I4" s="14"/>
-      <c r="J4" s="14"/>
-      <c r="K4" s="14"/>
-      <c r="L4" s="14"/>
-      <c r="M4" s="14"/>
-      <c r="N4" s="30"/>
+      <c r="B4" s="15"/>
+      <c r="C4" s="13"/>
+      <c r="D4" s="13"/>
+      <c r="E4" s="13"/>
+      <c r="F4" s="13"/>
+      <c r="G4" s="13"/>
+      <c r="H4" s="13"/>
+      <c r="I4" s="13"/>
+      <c r="J4" s="13"/>
+      <c r="K4" s="13"/>
+      <c r="L4" s="13"/>
+      <c r="M4" s="13"/>
+      <c r="N4" s="19"/>
       <c r="O4" s="2"/>
     </row>
     <row r="5" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B5" s="32"/>
-      <c r="C5" s="33" t="s">
+      <c r="B5" s="21"/>
+      <c r="C5" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="D5" s="14" t="s">
+      <c r="D5" s="23" t="s">
         <v>32</v>
       </c>
-      <c r="E5" s="14" t="s">
+      <c r="E5" s="23" t="s">
         <v>41</v>
       </c>
-      <c r="F5" s="14" t="s">
+      <c r="F5" s="23" t="s">
         <v>40</v>
       </c>
-      <c r="G5" s="14" t="s">
+      <c r="G5" s="23" t="s">
         <v>33</v>
       </c>
-      <c r="H5" s="14" t="s">
+      <c r="H5" s="23" t="s">
         <v>34</v>
       </c>
-      <c r="I5" s="14" t="s">
+      <c r="I5" s="23" t="s">
         <v>35</v>
       </c>
-      <c r="J5" s="14" t="s">
+      <c r="J5" s="23" t="s">
         <v>36</v>
       </c>
-      <c r="K5" s="14" t="s">
+      <c r="K5" s="23" t="s">
         <v>37</v>
       </c>
-      <c r="L5" s="14" t="s">
+      <c r="L5" s="23" t="s">
         <v>38</v>
       </c>
-      <c r="M5" s="29" t="s">
+      <c r="M5" s="24" t="s">
         <v>39</v>
       </c>
-      <c r="N5" s="31"/>
+      <c r="N5" s="20"/>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.3">
       <c r="C6" s="5"/>
@@ -1270,12 +1288,12 @@
       <c r="M6" s="5"/>
     </row>
     <row r="7" spans="1:17" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B7" s="19"/>
-      <c r="C7" s="26" t="s">
+      <c r="B7" s="17"/>
+      <c r="C7" s="31" t="s">
         <v>13</v>
       </c>
-      <c r="D7" s="26"/>
-      <c r="E7" s="20" t="s">
+      <c r="D7" s="31"/>
+      <c r="E7" s="18" t="s">
         <v>14</v>
       </c>
       <c r="F7" s="3"/>
@@ -1292,14 +1310,14 @@
       <c r="Q7" s="4"/>
     </row>
     <row r="8" spans="1:17" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="17" t="s">
+      <c r="B8" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="C8" s="24" t="s">
+      <c r="C8" s="29" t="s">
         <v>29</v>
       </c>
-      <c r="D8" s="25"/>
-      <c r="E8" s="18" t="s">
+      <c r="D8" s="30"/>
+      <c r="E8" s="34" t="s">
         <v>30</v>
       </c>
       <c r="F8" s="3"/>
@@ -1317,8 +1335,8 @@
     </row>
     <row r="9" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B9" s="6"/>
-      <c r="C9" s="27"/>
-      <c r="D9" s="28"/>
+      <c r="C9" s="32"/>
+      <c r="D9" s="33"/>
       <c r="E9" s="7"/>
     </row>
   </sheetData>

</xml_diff>